<commit_message>
add big category var
</commit_message>
<xml_diff>
--- a/field_names_validated.xlsx
+++ b/field_names_validated.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Documents\GitHub\shelter-exits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps4375\Documents\GitHub\shelter-exits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839E0DDD-F7E4-41F8-9071-90C420148D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="128">
   <si>
     <t>facility_or_program_type</t>
   </si>
@@ -398,12 +397,18 @@
   </si>
   <si>
     <t>DYCD only?</t>
+  </si>
+  <si>
+    <t>housing_category</t>
+  </si>
+  <si>
+    <t>Permanent Housing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -748,20 +753,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="156.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -772,10 +778,13 @@
         <v>108</v>
       </c>
       <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -788,8 +797,11 @@
       <c r="D2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -802,8 +814,11 @@
       <c r="D3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -816,8 +831,11 @@
       <c r="D4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -830,8 +848,11 @@
       <c r="D5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -844,8 +865,11 @@
       <c r="D6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -858,8 +882,11 @@
       <c r="D7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -872,8 +899,11 @@
       <c r="D8" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -886,8 +916,11 @@
       <c r="D9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -900,8 +933,11 @@
       <c r="D10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -915,10 +951,13 @@
         <v>64</v>
       </c>
       <c r="E11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -932,10 +971,13 @@
         <v>113</v>
       </c>
       <c r="E12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -948,8 +990,11 @@
       <c r="D13" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -962,8 +1007,11 @@
       <c r="D14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -976,8 +1024,11 @@
       <c r="D15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -990,8 +1041,11 @@
       <c r="D16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1004,8 +1058,11 @@
       <c r="D17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1018,8 +1075,11 @@
       <c r="D18" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1032,8 +1092,11 @@
       <c r="D19" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1046,8 +1109,11 @@
       <c r="D20" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1060,8 +1126,11 @@
       <c r="D21" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1074,8 +1143,11 @@
       <c r="D22" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1088,8 +1160,11 @@
       <c r="D23" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1103,10 +1178,13 @@
         <v>111</v>
       </c>
       <c r="E24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1119,8 +1197,11 @@
       <c r="D25" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1133,8 +1214,11 @@
       <c r="D26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1147,8 +1231,11 @@
       <c r="D27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1161,8 +1248,11 @@
       <c r="D28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1175,8 +1265,11 @@
       <c r="D29" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1189,8 +1282,11 @@
       <c r="D30" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1203,8 +1299,11 @@
       <c r="D31" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1218,10 +1317,13 @@
         <v>85</v>
       </c>
       <c r="E32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1235,10 +1337,13 @@
         <v>85</v>
       </c>
       <c r="E33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1251,8 +1356,11 @@
       <c r="D34" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1265,8 +1373,11 @@
       <c r="D35" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1279,8 +1390,11 @@
       <c r="D36" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1294,10 +1408,13 @@
         <v>85</v>
       </c>
       <c r="E37" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1311,10 +1428,13 @@
         <v>85</v>
       </c>
       <c r="E38" t="s">
+        <v>127</v>
+      </c>
+      <c r="F38" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1327,8 +1447,11 @@
       <c r="D39" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1341,8 +1464,11 @@
       <c r="D40" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1355,8 +1481,11 @@
       <c r="D41" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1369,8 +1498,11 @@
       <c r="D42" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1383,8 +1515,11 @@
       <c r="D43" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1397,8 +1532,11 @@
       <c r="D44" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1411,8 +1549,11 @@
       <c r="D45" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1425,8 +1566,11 @@
       <c r="D46" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1439,8 +1583,11 @@
       <c r="D47" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1454,10 +1601,13 @@
         <v>69</v>
       </c>
       <c r="E48" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1470,8 +1620,11 @@
       <c r="D49" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1484,8 +1637,11 @@
       <c r="D50" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1498,8 +1654,11 @@
       <c r="D51" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1512,8 +1671,11 @@
       <c r="D52" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1526,8 +1688,11 @@
       <c r="D53" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1541,6 +1706,9 @@
         <v>69</v>
       </c>
       <c r="E54" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>